<commit_message>
Changed Read Logic for Outputsettings
</commit_message>
<xml_diff>
--- a/DataExtractionTool/DataExtractionTool/bin/Debug/Input.xlsx
+++ b/DataExtractionTool/DataExtractionTool/bin/Debug/Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m87316\source\repos\DataExtractionTool\DataExtractionTool\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m87316\Documents\GitHub\BIDataExtractTool\DataExtractionTool\DataExtractionTool\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEEFDB7-6505-43F6-862B-402A0BD2149D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890962B1-30AF-4C54-9596-49BB6E549A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229DDE17-1B62-4C2E-8665-3187265BABD1}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3200,7 +3200,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -3366,13 +3366,13 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3839,7 +3839,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3939,7 +3939,7 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -3947,19 +3947,19 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>43952</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>44075</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -9145,10 +9145,10 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>43831</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>44075</v>
       </c>
       <c r="E2" t="s">
@@ -9186,6 +9186,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007FFA6BD16B38B84F92EC25882A5E8E80" ma:contentTypeVersion="6" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="0b72efba560537ea172084cd8b44b582">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5d540d49-f4f6-404c-8b70-49c42e676c52" xmlns:ns4="d76e8a69-b40a-48cd-ab2d-90e1659f6357" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51556ea69bf20cb8fd8cd3a759762477" ns3:_="" ns4:_="">
     <xsd:import namespace="5d540d49-f4f6-404c-8b70-49c42e676c52"/>
@@ -9362,15 +9371,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -9378,6 +9378,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3459CC55-32AF-44F2-8402-05F01F7D5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEDD452E-885B-4FE9-9F77-D499AEC2253A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9392,14 +9400,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3459CC55-32AF-44F2-8402-05F01F7D5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>